<commit_message>
Make the JSON not suck
</commit_message>
<xml_diff>
--- a/backend/copysheet.xlsx
+++ b/backend/copysheet.xlsx
@@ -14,7 +14,7 @@
     <sheet name="University Unions (Unions)" sheetId="5" r:id="rId5"/>
     <sheet name="metadata" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="135">
   <si>
     <t>Candidate Name</t>
   </si>
@@ -89,492 +89,309 @@
     <t>Rohit Mandalapu</t>
   </si>
   <si>
-    <t>Executive Alliance</t>
-  </si>
-  <si>
     <t>Vice President</t>
   </si>
   <si>
     <t>Plan II/Economics</t>
   </si>
   <si>
-    <t>Senior</t>
-  </si>
-  <si>
     <t>Braydon Jones</t>
   </si>
   <si>
-    <t>Executive Alliance</t>
-  </si>
-  <si>
-    <t>President</t>
-  </si>
-  <si>
     <t>Government/LAH</t>
   </si>
   <si>
-    <t>Senior</t>
-  </si>
-  <si>
     <t>https://twitter.com/braydon_jones</t>
   </si>
   <si>
-    <t>Candidate Name</t>
-  </si>
-  <si>
-    <t>Candidate Name</t>
-  </si>
-  <si>
-    <t>Category Number</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Subcategory</t>
-  </si>
-  <si>
-    <t>Photo URL</t>
-  </si>
-  <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>Photo Credit</t>
-  </si>
-  <si>
-    <t>Major</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Statement</t>
-  </si>
-  <si>
-    <t>Campaign Platform Points</t>
-  </si>
-  <si>
-    <t>Twitter Feed URL</t>
-  </si>
-  <si>
-    <t>Campaign Website</t>
-  </si>
-  <si>
-    <t>Daily Texan Coverage Titles</t>
-  </si>
-  <si>
-    <t>Daily Texan Coverage URLs</t>
+    <t>Kimia Dargahi</t>
+  </si>
+  <si>
+    <t>International Relations &amp; Global Studies/LAH</t>
+  </si>
+  <si>
+    <t>Kallen Dimitroff</t>
+  </si>
+  <si>
+    <t>University-Wide Representatives</t>
+  </si>
+  <si>
+    <t>University-Wide Representative</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>Junior</t>
+  </si>
+  <si>
+    <t>Kevin Helgren</t>
+  </si>
+  <si>
+    <t>Psychology/Neuroscience</t>
+  </si>
+  <si>
+    <t>Conlee Hamlin</t>
+  </si>
+  <si>
+    <t>Nutrition</t>
+  </si>
+  <si>
+    <t>Freshman</t>
+  </si>
+  <si>
+    <t>https://twitter.com/conlee_hamlin</t>
+  </si>
+  <si>
+    <t>Spencer Schredder</t>
+  </si>
+  <si>
+    <t>International Relations &amp; Global Studies</t>
+  </si>
+  <si>
+    <t>John Falke</t>
+  </si>
+  <si>
+    <t>BHP/Finance/Government</t>
+  </si>
+  <si>
+    <t>Sophomore</t>
+  </si>
+  <si>
+    <t>Santiago Rosales</t>
+  </si>
+  <si>
+    <t>Ryan Lim</t>
+  </si>
+  <si>
+    <t>http://i.imgur.com/bPntGgD.jpg</t>
+  </si>
+  <si>
+    <t>Courtesy</t>
+  </si>
+  <si>
+    <t>Hi I’m Ryan Lim and I’m here to challenge the perception on campus of what student government means. As the social chair for the Pi Kappa Phi Fraternity, I’ve learned some things. First, THE University of Texas has an astonishing amount of great people with different beliefs and ideas that should be embraced. Second, simply how to have fun. Though we all know that the most important reason to go to college is to get an education, that doesn’t mean college shouldn’t be fun. Though our Student Government has done great work for our university, do you feel that they are representative of you? You may see me in Professor Bonevac’s class or at Gregory, but you can also catch me at Blind Pig or at Roundup. Government should represent you, plain and simple. I believe that I am for the people and soon to be by the people.</t>
+  </si>
+  <si>
+    <t>Represent the UT community at large, with emphasis on those felt disenfranchised by the current system|||Act only on behalf of the Student population|||Oppose any legislation that infringes on the rights of Students|||Endeavor to bring West Campus back to its former Glory|||Maintain the notion that UT is the best place to attend college.</t>
+  </si>
+  <si>
+    <t>Valentina Rodriguez</t>
+  </si>
+  <si>
+    <t>College Representatives</t>
+  </si>
+  <si>
+    <t>Architecture Representative</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>Brian Schwall</t>
+  </si>
+  <si>
+    <t>Communication Representatives</t>
+  </si>
+  <si>
+    <t>Communication Representative</t>
+  </si>
+  <si>
+    <t>Corporate Communication Studies</t>
+  </si>
+  <si>
+    <t>https://twitter.com/iceman81894</t>
+  </si>
+  <si>
+    <t>Allison Ainsworth</t>
+  </si>
+  <si>
+    <t>Political communication</t>
+  </si>
+  <si>
+    <t>Bronwyn Baker</t>
+  </si>
+  <si>
+    <t>Education Representative</t>
+  </si>
+  <si>
+    <t>Applied Learning &amp; Development</t>
+  </si>
+  <si>
+    <t>Edward A. Banner</t>
+  </si>
+  <si>
+    <t>Engineering Representatives</t>
+  </si>
+  <si>
+    <t>Engineering Representative</t>
+  </si>
+  <si>
+    <t>Petroleum Engineering</t>
+  </si>
+  <si>
+    <t>Joshua Richardson</t>
+  </si>
+  <si>
+    <t>http://i.imgur.com/N7DiqI5.jpg</t>
+  </si>
+  <si>
+    <t>Electrical and Computer Engineering</t>
+  </si>
+  <si>
+    <t>When it comes to visions for the engineering student body, I cannot say that I have some grand overarching scheme that I wish to begin implementing right off the bat. Generally, if engineers have a problem, I think it’s safe to say we just hunker down and push through it, willing to persist through the challenge, be it large or small. That being said, I do have a few ideas involving implementation of better systems to make students more aware of help and resources which often fly under the radar; primarily, however, my goal is to have as tight of a feedback loop with students as possible, bringing their ideas to the table, and even if solutions to them are not possible through means which I have access to, at least bringing plausible issues to light.</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/joshua.richardson.1293</t>
+  </si>
+  <si>
+    <t>Lauren Gusman</t>
+  </si>
+  <si>
+    <t>Fine Arts Representative</t>
+  </si>
+  <si>
+    <t>http://i.imgur.com/KDvT8n9.jpg</t>
+  </si>
+  <si>
+    <t>Vocal performance/music</t>
+  </si>
+  <si>
+    <t>Hey Fine Arts Longhorns! My name is Lauren Gusman and I am a Vocal Performance major in the Butler School of Music. I am running to be your Fine Arts Representative for the upcoming school year. Although I am a first year, I have found my though some wonderful leadership programs such as the University Leadership Network, Gateway Scholars, The Multicultural Leadership Institute, Phi Beta Chi (A Professional Women’s Business Organization), and I am the Vice President of Music in the Fine Arts Council. Through these programs, I have learned to strive for excellence, exemplify team building, and gain character. I have noticed as I have been here, as far as the Fine Arts college goes, we have fallen behind. We’ve lost some of our best programs from all three of our departments. University wide, this was a loss. While I can’t say I can bring those back, I do plan on having a come back. Given this, it’s time we come together as a college to work together to overcome our losses. As the Student Government Fine Arts Representative, my visions for us is to communicate. Through our commeradery and our basic need of creativity, I plan on building more programs and clubs inside our college based on what our fine arts student body wants as a whole. From academics to performances to art galleries, I care about our image. I don’t just want to be the voice for all of us, I want to be the voice y’all choose to represent who we are and what we can do. Feel free to ask me any questions in person or by email: laurenagusman@utexas.edu.</t>
+  </si>
+  <si>
+    <t>James Che</t>
+  </si>
+  <si>
+    <t>Geosciences Representative</t>
+  </si>
+  <si>
+    <t>Geological Sciences</t>
+  </si>
+  <si>
+    <t>Kevin Toth</t>
+  </si>
+  <si>
+    <t>Kian Maharaj</t>
+  </si>
+  <si>
+    <t>Daniel Hung</t>
+  </si>
+  <si>
+    <t>Law Representative</t>
+  </si>
+  <si>
+    <t>http://i.imgur.com/JmnsdZC.jpg</t>
+  </si>
+  <si>
+    <t>Law</t>
+  </si>
+  <si>
+    <t>First year</t>
+  </si>
+  <si>
+    <t>I am running for SG Representative for the Law School, because I believe in serving others. Having attended UT since 2010 and graduating last year with a B.A. in Plan II Honors, Government Honors, History, and Asian Studies, I have more experience on campus than nearly all the other candidates. In addition, I have previous experience in SG as the Director of Students with Disabilities Agency from 2011-2012 and serving on the Parking &amp; Traffic Appeals Committee from 2013-2014. As SG Rep, I would be representing a population of UT students that haven’t been represented in SG in the last few years and will work towards increasing law students’ involvement with the rest of the campus. In this capacity, I will also be able to address any concerns law students may have through passing resolutions and working with the different university administrations.</t>
+  </si>
+  <si>
+    <t>Advocate for keeping tuition low|||Promote transparency in SG and UT|||Reach out to groups historically neglected by SG|||Connect law students with the rest of the University|||Push for abandoning affirmative action|||Ensure fair and public debates on resolutions|||Educate students on the roles of SG and UT|||Work towards making UT safer|||Make UT a more enjoyable place for everyone|||Foster peaceful and open dialogue on contentious issues</t>
+  </si>
+  <si>
+    <t>Tanner Long</t>
+  </si>
+  <si>
+    <t>Liberal Arts Representatives</t>
+  </si>
+  <si>
+    <t>Liberal Arts Representative</t>
+  </si>
+  <si>
+    <t>My name is Tanner Long and I’m running for reelection to be one of four representatives for the College of Liberal Arts. This past year, I’ve worked on numerous issues ranging from student input regarding the West Campus sound ordinance to more Monday-Wednesday classes to keeping the FAC open 24/7. Although my term is nearing the end, I still have not accomplished all the goals I’ve sought. Another year of being a Liberal Arts Representative will allow me to pursue more issues and provide you all with an experienced voice in the assembly. I will continue to focus on improving student engagement, voicing concerns of students to Austin City Hall, the Texas State Legislature and the U.S. Congress, and adequately represent the opinion of Liberal Arts students.</t>
+  </si>
+  <si>
+    <t>twitter.com/TannerLLong</t>
+  </si>
+  <si>
+    <t>Connor Madden</t>
+  </si>
+  <si>
+    <t>Plan II/Business</t>
+  </si>
+  <si>
+    <t>twitter.com/votemadden</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/connor.madden.73</t>
+  </si>
+  <si>
+    <t>Shawn A. Lopez</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Hello, my name is Shawn Lopez and I’m running for college of liberal arts representative. My campaign will be run on a platform of honest initiative in which I hold the goal of bringing to light all the issues concerning students within the COLA; these issues range from affordability to assessment challenges that I will personally look to improve if elected to a term as your representative. The solutions are clear and can be instituted through my advocacy if elected, but only if you are willing to follow me through and help me accomplish what needs to be done in the process. As I will show in my campaign, I am here as a voice through which yours will be spoken and your grievances brought to light. I am your candidate and hope to be your future voice in student government.</t>
+  </si>
+  <si>
+    <t>College affordability|||Increase in student study resources|||Advocate of Student safety|||Fight for student rights|||Make student government more accessible to the student body</t>
+  </si>
+  <si>
+    <t>James Comer</t>
+  </si>
+  <si>
+    <t>Economics</t>
+  </si>
+  <si>
+    <t>Sammy Minkowitz</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/sammy.minkowitz</t>
+  </si>
+  <si>
+    <t>Jonathan Dror</t>
+  </si>
+  <si>
+    <t>John-Paul Bach</t>
+  </si>
+  <si>
+    <t>Natural Sciences Representatives</t>
+  </si>
+  <si>
+    <t>Natural Sciences Representative</t>
+  </si>
+  <si>
+    <t>Biology</t>
+  </si>
+  <si>
+    <t>Juan Saez</t>
+  </si>
+  <si>
+    <t>Undergraduate Studies Representative</t>
+  </si>
+  <si>
+    <t>Undeclared</t>
+  </si>
+  <si>
+    <t>Establish mentorship programs for new UGS and PACE students (seperate programs).|||Develop a comprehensive and official website for PACE students for them to visit for information.|||Increase student participation in SG elections via incentives in order to guarantee fair representation.|||Improve the connection between SG representatives and the student population through social media and public meetings.|||Raise campus-wide awareness of important global issues.|||Promote UGS student participation in University-run or University-endorsed events and organizations.</t>
   </si>
   <si>
     <t>Brian Wilkey</t>
   </si>
   <si>
-    <t>Category Number</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Subcategory</t>
-  </si>
-  <si>
-    <t>Photo URL</t>
-  </si>
-  <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>Photo Credit</t>
-  </si>
-  <si>
-    <t>Major</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Statement</t>
-  </si>
-  <si>
-    <t>Campaign Platform Points</t>
-  </si>
-  <si>
-    <t>Twitter Feed URL</t>
-  </si>
-  <si>
-    <t>Campaign Website</t>
-  </si>
-  <si>
-    <t>Daily Texan Coverage Titles</t>
-  </si>
-  <si>
-    <t>Daily Texan Coverage URLs</t>
-  </si>
-  <si>
     <t>Graduate Student Assembly President</t>
   </si>
   <si>
-    <t>Candidate Name</t>
-  </si>
-  <si>
-    <t>President</t>
-  </si>
-  <si>
-    <t>Category Number</t>
-  </si>
-  <si>
     <t>Human Development &amp; Family Sciences</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Subcategory</t>
-  </si>
-  <si>
     <t>Vance Roper</t>
   </si>
   <si>
-    <t>Photo URL</t>
-  </si>
-  <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>Photo Credit</t>
-  </si>
-  <si>
-    <t>Major</t>
-  </si>
-  <si>
     <t>Graduate Student Assembly Vice President</t>
   </si>
   <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Statement</t>
-  </si>
-  <si>
-    <t>Vice President</t>
-  </si>
-  <si>
-    <t>Campaign Platform Points</t>
-  </si>
-  <si>
     <t>Public Affairs/Community and Regional Planning</t>
   </si>
   <si>
-    <t>Twitter Feed URL</t>
-  </si>
-  <si>
-    <t>Campaign Website</t>
-  </si>
-  <si>
-    <t>Daily Texan Coverage Titles</t>
-  </si>
-  <si>
-    <t>Daily Texan Coverage URLs</t>
-  </si>
-  <si>
-    <t>Kimia Dargahi</t>
-  </si>
-  <si>
-    <t>Executive Alliance</t>
-  </si>
-  <si>
-    <t>Vice President</t>
-  </si>
-  <si>
-    <t>International Relations &amp; Global Studies/LAH</t>
-  </si>
-  <si>
-    <t>Senior</t>
-  </si>
-  <si>
-    <t>Kallen Dimitroff</t>
-  </si>
-  <si>
-    <t>University-Wide Representatives</t>
-  </si>
-  <si>
-    <t>University-Wide Representative</t>
-  </si>
-  <si>
-    <t>Government</t>
-  </si>
-  <si>
-    <t>Junior</t>
-  </si>
-  <si>
-    <t>Kevin Helgren</t>
-  </si>
-  <si>
-    <t>University-Wide Representatives</t>
-  </si>
-  <si>
-    <t>University-Wide Representative</t>
-  </si>
-  <si>
-    <t>Psychology/Neuroscience</t>
-  </si>
-  <si>
-    <t>Senior</t>
-  </si>
-  <si>
-    <t>Conlee Hamlin</t>
-  </si>
-  <si>
-    <t>University-Wide Representatives</t>
-  </si>
-  <si>
-    <t>University-Wide Representative</t>
-  </si>
-  <si>
-    <t>Nutrition</t>
-  </si>
-  <si>
-    <t>Freshman</t>
-  </si>
-  <si>
-    <t>https://twitter.com/conlee_hamlin</t>
-  </si>
-  <si>
-    <t>Spencer Schredder</t>
-  </si>
-  <si>
-    <t>University-Wide Representatives</t>
-  </si>
-  <si>
-    <t>University-Wide Representative</t>
-  </si>
-  <si>
-    <t>International Relations &amp; Global Studies</t>
-  </si>
-  <si>
-    <t>Junior</t>
-  </si>
-  <si>
-    <t>John Falke</t>
-  </si>
-  <si>
-    <t>University-Wide Representatives</t>
-  </si>
-  <si>
-    <t>University-Wide Representative</t>
-  </si>
-  <si>
-    <t>BHP/Finance/Government</t>
-  </si>
-  <si>
-    <t>Sophomore</t>
-  </si>
-  <si>
-    <t>Santiago Rosales</t>
-  </si>
-  <si>
-    <t>University-Wide Representatives</t>
-  </si>
-  <si>
-    <t>University-Wide Representative</t>
-  </si>
-  <si>
-    <t>Ryan Lim</t>
-  </si>
-  <si>
-    <t>University-Wide Representatives</t>
-  </si>
-  <si>
-    <t>http://i.imgur.com/bPntGgD.jpg</t>
-  </si>
-  <si>
-    <t>University-Wide Representative</t>
-  </si>
-  <si>
-    <t>Government</t>
-  </si>
-  <si>
-    <t>Junior</t>
-  </si>
-  <si>
-    <t>Hi I’m Ryan Lim and I’m here to challenge the perception on campus of what student government means. As the social chair for the Pi Kappa Phi Fraternity, I’ve learned some things. First, THE University of Texas has an astonishing amount of great people with different beliefs and ideas that should be embraced. Second, simply how to have fun. Though we all know that the most important reason to go to college is to get an education, that doesn’t mean college shouldn’t be fun. Though our Student Government has done great work for our university, do you feel that they are representative of you? You may see me in Professor Bonevac’s class or at Gregory, but you can also catch me at Blind Pig or at Roundup. Government should represent you, plain and simple. I believe that I am for the people and soon to be by the people.</t>
-  </si>
-  <si>
-    <t>Represent the UT community at large, with emphasis on those felt disenfranchised by the current system|||Act only on behalf of the Student population|||Oppose any legislation that infringes on the rights of Students|||Endeavor to bring West Campus back to its former Glory|||Maintain the notion that UT is the best place to attend college.</t>
-  </si>
-  <si>
-    <t>Valentina Rodriguez</t>
-  </si>
-  <si>
-    <t>College Representatives</t>
-  </si>
-  <si>
-    <t>Architecture Representative</t>
-  </si>
-  <si>
-    <t>Architecture Representative</t>
-  </si>
-  <si>
-    <t>Architecture</t>
-  </si>
-  <si>
-    <t>Sophomore</t>
-  </si>
-  <si>
-    <t>Brian Schwall</t>
-  </si>
-  <si>
-    <t>College Representatives</t>
-  </si>
-  <si>
-    <t>Communication Representatives</t>
-  </si>
-  <si>
-    <t>Communication Representative</t>
-  </si>
-  <si>
-    <t>Corporate Communication Studies</t>
-  </si>
-  <si>
-    <t>Junior</t>
-  </si>
-  <si>
-    <t>https://twitter.com/iceman81894</t>
-  </si>
-  <si>
-    <t>Candidate Name</t>
-  </si>
-  <si>
-    <t>Category Number</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Subcategory</t>
-  </si>
-  <si>
-    <t>Photo URL</t>
-  </si>
-  <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>Photo Credit</t>
-  </si>
-  <si>
-    <t>Major</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Statement</t>
-  </si>
-  <si>
-    <t>Campaign Platform Points</t>
-  </si>
-  <si>
-    <t>Twitter Feed URL</t>
-  </si>
-  <si>
-    <t>Campaign Website</t>
-  </si>
-  <si>
-    <t>Allison Ainsworth</t>
-  </si>
-  <si>
-    <t>Daily Texan Coverage Titles</t>
-  </si>
-  <si>
-    <t>Daily Texan Coverage URLs</t>
-  </si>
-  <si>
-    <t>College Representatives</t>
-  </si>
-  <si>
-    <t>Communication Representatives</t>
-  </si>
-  <si>
-    <t>Communication Representative</t>
-  </si>
-  <si>
-    <t>Bronwyn Baker</t>
-  </si>
-  <si>
-    <t>College Representatives</t>
-  </si>
-  <si>
-    <t>Education Representative</t>
-  </si>
-  <si>
-    <t>Education Representative</t>
-  </si>
-  <si>
-    <t>Applied Learning &amp; Development</t>
-  </si>
-  <si>
-    <t>Sophomore</t>
-  </si>
-  <si>
-    <t>Edward A. Banner</t>
-  </si>
-  <si>
-    <t>College Representatives</t>
-  </si>
-  <si>
-    <t>Engineering Representatives</t>
-  </si>
-  <si>
-    <t>Engineering Representative</t>
-  </si>
-  <si>
-    <t>Petroleum Engineering</t>
-  </si>
-  <si>
-    <t>Junior</t>
-  </si>
-  <si>
-    <t>Joshua Richardson</t>
-  </si>
-  <si>
-    <t>College Representatives</t>
-  </si>
-  <si>
-    <t>Engineering Representatives</t>
-  </si>
-  <si>
-    <t>http://i.imgur.com/N7DiqI5.jpg</t>
-  </si>
-  <si>
-    <t>Engineering Representative</t>
-  </si>
-  <si>
-    <t>Electrical and Computer Engineering</t>
-  </si>
-  <si>
-    <t>Sophomore</t>
-  </si>
-  <si>
-    <t>When it comes to visions for the engineering student body, I cannot say that I have some grand overarching scheme that I wish to begin implementing right off the bat. Generally, if engineers have a problem, I think it’s safe to say we just hunker down and push through it, willing to persist through the challenge, be it large or small. That being said, I do have a few ideas involving implementation of better systems to make students more aware of help and resources which often fly under the radar; primarily, however, my goal is to have as tight of a feedback loop with students as possible, bringing their ideas to the table, and even if solutions to them are not possible through means which I have access to, at least bringing plausible issues to light.</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/joshua.richardson.1293</t>
-  </si>
-  <si>
-    <t>Lauren Gusman</t>
-  </si>
-  <si>
-    <t>College Representatives</t>
-  </si>
-  <si>
-    <t>Fine Arts Representative</t>
-  </si>
-  <si>
-    <t>http://i.imgur.com/KDvT8n9.jpg</t>
-  </si>
-  <si>
     <t>key</t>
   </si>
   <si>
@@ -584,278 +401,41 @@
     <t>Student Government (SG)</t>
   </si>
   <si>
+    <t>Student Government is the official student voice to the UT administration, the Board of Regents and the Texas Legislature. SG aims to represent students' interests and increase student decision-making power and to improve campus life by creating and continuing effective student services. Members of the organization write resolutions voicing their support or disapproval of certain University, UT System or legislative actions; proposing new ideas; and formally addressing student concerns. Members can also make internal changes to Student Government, including the Election Code, which candidates for the body must follow every year.|||The president and vice president, known as the executive alliance, lead the executive branch of Student Government. The chair of the assembly leads the legislative branch of Student Government, and the chief justice leads the judicial branch of Student Government. These branches include various committees and agencies. The student body elects the president and vice president, who run on one ticket; eight university-wide representatives; and representatives for each of 16 schools and colleges within the University. The Dell Medical School, which will accept its first class in August 2016, and the School of Information do not currently have representative positions in Student Government. The graduate school has four representatives in Student Government.</t>
+  </si>
+  <si>
     <t>Graduate Student Assembly (GSA)</t>
   </si>
   <si>
+    <t>Graduate Student Assembly is the official graduate student voice to the UT administration, the Board of Regents and the Texas Legislature. Members of the organization write resolutions voicing their support or disapproval of certain University, UT System or legislative actions; proposing new ideas; and formally addressing graduate student concerns. The graduate student body elects a president and vice president, who lead the executive committee. The executive committee consists of various directors, who are approved by 2/3 of the Graduate Student Assembly.</t>
+  </si>
+  <si>
     <t>Texas Student Media (TSM)</t>
   </si>
   <si>
+    <t>The Texas Student Media Operating Board of Trustees oversees the University's five official media outlets: KVRX 91.7 FM, the Texas Travesty, Texas Student Television, the Cactus yearbook and The Daily Texan. The student body elects three Moody College of Communication students and three at-large students to the board. The University president appoints two members of the Moody College of Communication faculty, one member of the McCombs School of Business faculty and two media professionals. These members are all voting members. The non-voting members are the TSM director, the student managers of the five TSM entities, the TSM student advertising director, a Dean of Students Office representative and a Student Government representative.|||The organization oversees the TSM budget; appoints the student managers of the TSM entities (except The Daily Texan editor-in-chief, who is elected by the student body); supervises the student managers of the TSM entities. The TSM board reports to the UT System Board of Regents.</t>
+  </si>
+  <si>
     <t>University Co-Op (Co-Op)</t>
   </si>
   <si>
+    <t>The University Co-op Board of Directors directs the University Co-op and oversees scholarships, grants and funding. The board consists of four students, four faculty members, two independent members and a chair. The student body elects two full-time students to serve on the board for two years. Everyone on the board is a voting member.</t>
+  </si>
+  <si>
     <t>University Unions (Unions)</t>
   </si>
   <si>
-    <t>Fine Arts Representative</t>
-  </si>
-  <si>
-    <t>Vocal performance/music</t>
-  </si>
-  <si>
-    <t>Sophomore</t>
-  </si>
-  <si>
-    <t>Hey Fine Arts Longhorns! My name is Lauren Gusman and I am a Vocal Performance major in the Butler School of Music. I am running to be your Fine Arts Representative for the upcoming school year. Although I am a first year, I have found my though some wonderful leadership programs such as the University Leadership Network, Gateway Scholars, The Multicultural Leadership Institute, Phi Beta Chi (A Professional Women’s Business Organization), and I am the Vice President of Music in the Fine Arts Council. Through these programs, I have learned to strive for excellence, exemplify team building, and gain character. I have noticed as I have been here, as far as the Fine Arts college goes, we have fallen behind. We’ve lost some of our best programs from all three of our departments. University wide, this was a loss. While I can’t say I can bring those back, I do plan on having a come back. Given this, it’s time we come together as a college to work together to overcome our losses. As the Student Government Fine Arts Representative, my visions for us is to communicate. Through our commeradery and our basic need of creativity, I plan on building more programs and clubs inside our college based on what our fine arts student body wants as a whole. From academics to performances to art galleries, I care about our image. I don’t just want to be the voice for all of us, I want to be the voice y’all choose to represent who we are and what we can do. Feel free to ask me any questions in person or by email: laurenagusman@utexas.edu.</t>
-  </si>
-  <si>
-    <t>James Che</t>
-  </si>
-  <si>
-    <t>College Representatives</t>
-  </si>
-  <si>
-    <t>Geosciences Representative</t>
-  </si>
-  <si>
-    <t>Geosciences Representative</t>
-  </si>
-  <si>
-    <t>Geological Sciences</t>
-  </si>
-  <si>
-    <t>Junior</t>
-  </si>
-  <si>
-    <t>Kevin Toth</t>
-  </si>
-  <si>
-    <t>College Representatives</t>
-  </si>
-  <si>
-    <t>Geosciences Representative</t>
-  </si>
-  <si>
-    <t>Geosciences Representative</t>
-  </si>
-  <si>
-    <t>Geological Sciences</t>
-  </si>
-  <si>
-    <t>Junior</t>
-  </si>
-  <si>
-    <t>Kian Maharaj</t>
-  </si>
-  <si>
-    <t>College Representatives</t>
-  </si>
-  <si>
-    <t>Geosciences Representative</t>
-  </si>
-  <si>
-    <t>Geosciences Representative</t>
-  </si>
-  <si>
-    <t>Geological Sciences</t>
-  </si>
-  <si>
-    <t>Sophomore</t>
-  </si>
-  <si>
-    <t>Daniel Hung</t>
-  </si>
-  <si>
-    <t>College Representatives</t>
-  </si>
-  <si>
-    <t>Law Representative</t>
-  </si>
-  <si>
-    <t>http://i.imgur.com/JmnsdZC.jpg</t>
-  </si>
-  <si>
-    <t>Law Representative</t>
-  </si>
-  <si>
-    <t>Law</t>
-  </si>
-  <si>
-    <t>First year</t>
-  </si>
-  <si>
-    <t>I am running for SG Representative for the Law School, because I believe in serving others. Having attended UT since 2010 and graduating last year with a B.A. in Plan II Honors, Government Honors, History, and Asian Studies, I have more experience on campus than nearly all the other candidates. In addition, I have previous experience in SG as the Director of Students with Disabilities Agency from 2011-2012 and serving on the Parking &amp; Traffic Appeals Committee from 2013-2014. As SG Rep, I would be representing a population of UT students that haven’t been represented in SG in the last few years and will work towards increasing law students’ involvement with the rest of the campus. In this capacity, I will also be able to address any concerns law students may have through passing resolutions and working with the different university administrations.</t>
-  </si>
-  <si>
-    <t>Advocate for keeping tuition low|||Promote transparency in SG and UT|||Reach out to groups historically neglected by SG|||Connect law students with the rest of the University|||Push for abandoning affirmative action|||Ensure fair and public debates on resolutions|||Educate students on the roles of SG and UT|||Work towards making UT safer|||Make UT a more enjoyable place for everyone|||Foster peaceful and open dialogue on contentious issues</t>
-  </si>
-  <si>
-    <t>Tanner Long</t>
-  </si>
-  <si>
-    <t>College Representatives</t>
-  </si>
-  <si>
-    <t>Liberal Arts Representatives</t>
-  </si>
-  <si>
-    <t>Liberal Arts Representative</t>
-  </si>
-  <si>
-    <t>Government</t>
-  </si>
-  <si>
-    <t>Junior</t>
-  </si>
-  <si>
-    <t>My name is Tanner Long and I’m running for reelection to be one of four representatives for the College of Liberal Arts. This past year, I’ve worked on numerous issues ranging from student input regarding the West Campus sound ordinance to more Monday-Wednesday classes to keeping the FAC open 24/7. Although my term is nearing the end, I still have not accomplished all the goals I’ve sought. Another year of being a Liberal Arts Representative will allow me to pursue more issues and provide you all with an experienced voice in the assembly. I will continue to focus on improving student engagement, voicing concerns of students to Austin City Hall, the Texas State Legislature and the U.S. Congress, and adequately represent the opinion of Liberal Arts students.</t>
-  </si>
-  <si>
-    <t>twitter.com/TannerLLong</t>
-  </si>
-  <si>
-    <t>Connor Madden</t>
-  </si>
-  <si>
-    <t>College Representatives</t>
-  </si>
-  <si>
-    <t>Liberal Arts Representatives</t>
-  </si>
-  <si>
-    <t>Liberal Arts Representative</t>
-  </si>
-  <si>
-    <t>Plan II/Business</t>
-  </si>
-  <si>
-    <t>Sophomore</t>
-  </si>
-  <si>
-    <t>Shawn A. Lopez</t>
-  </si>
-  <si>
-    <t>College Representatives</t>
-  </si>
-  <si>
-    <t>Liberal Arts Representatives</t>
-  </si>
-  <si>
-    <t>Liberal Arts Representative</t>
-  </si>
-  <si>
-    <t>History</t>
-  </si>
-  <si>
-    <t>Junior</t>
-  </si>
-  <si>
-    <t>James Comer</t>
-  </si>
-  <si>
-    <t>College Representatives</t>
-  </si>
-  <si>
-    <t>Liberal Arts Representatives</t>
-  </si>
-  <si>
-    <t>Liberal Arts Representative</t>
-  </si>
-  <si>
-    <t>Economics</t>
-  </si>
-  <si>
-    <t>Sophomore</t>
-  </si>
-  <si>
-    <t>Sammy Minkowitz</t>
-  </si>
-  <si>
-    <t>College Representatives</t>
-  </si>
-  <si>
-    <t>Liberal Arts Representatives</t>
-  </si>
-  <si>
-    <t>Liberal Arts Representative</t>
-  </si>
-  <si>
-    <t>Government</t>
-  </si>
-  <si>
-    <t>Freshman</t>
-  </si>
-  <si>
-    <t>Jonathan Dror</t>
-  </si>
-  <si>
-    <t>College Representatives</t>
-  </si>
-  <si>
-    <t>Liberal Arts Representatives</t>
-  </si>
-  <si>
-    <t>Liberal Arts Representative</t>
-  </si>
-  <si>
-    <t>Economics</t>
-  </si>
-  <si>
-    <t>Sophomore</t>
-  </si>
-  <si>
-    <t>John-Paul Bach</t>
-  </si>
-  <si>
-    <t>College Representatives</t>
-  </si>
-  <si>
-    <t>Natural Sciences Representatives</t>
-  </si>
-  <si>
-    <t>Natural Sciences Representative</t>
-  </si>
-  <si>
-    <t>Biology</t>
-  </si>
-  <si>
-    <t>Sophomore</t>
-  </si>
-  <si>
-    <t>Juan Saez</t>
-  </si>
-  <si>
-    <t>College Representatives</t>
-  </si>
-  <si>
-    <t>Undergraduate Studies Representative</t>
-  </si>
-  <si>
-    <t>Undergraduate Studies Representative</t>
-  </si>
-  <si>
-    <t>Undeclared</t>
-  </si>
-  <si>
-    <t>Freshman</t>
-  </si>
-  <si>
-    <t>Test1|||Test2</t>
-  </si>
-  <si>
-    <t>http://www.google.com|||http://www.reddit.com</t>
-  </si>
-  <si>
-    <t>Elly Dearman</t>
-  </si>
-  <si>
-    <t>http://www.TannerLong.com/</t>
+    <t>The University Unions Board of Directors recommend rules and procedures regarding the operation and use of the Unions' facilities, which include the Texas Union, the Student Activity Center and the Hogg Auditorium. The board also oversees Campus Events and Entertainment. The student body elects the Campus Events and Entertainment president and two students to serve on the board. The University president appoints three faculty members to the board. Additionally, the Student Government president and two students appointed by the SG president serve on the board. The board also contains two non-voting members: the representative of the Vice President for Student Affairs and the University Unions Executive Director.</t>
+  </si>
+  <si>
+    <t>http://www.TannerLong.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -875,15 +455,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -899,6 +470,21 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -940,7 +526,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -948,17 +534,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1294,10 +880,10 @@
   <dimension ref="A1:O66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1389,19 +975,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="2"/>
@@ -1412,30 +998,30 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="8" t="s">
-        <v>30</v>
+      <c r="L4" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
@@ -1443,25 +1029,25 @@
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>85</v>
+        <v>16</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="3" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="3" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="2"/>
@@ -1472,25 +1058,25 @@
     </row>
     <row r="6" spans="1:15" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>89</v>
+        <v>28</v>
       </c>
       <c r="B6" s="3">
         <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>90</v>
+        <v>29</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="3" t="s">
-        <v>91</v>
+        <v>30</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="3" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="2"/>
@@ -1501,25 +1087,25 @@
     </row>
     <row r="7" spans="1:15" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="B7" s="3">
         <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>95</v>
+        <v>29</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="3" t="s">
-        <v>96</v>
+        <v>30</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="3" t="s">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>98</v>
+        <v>19</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="2"/>
@@ -1530,30 +1116,30 @@
     </row>
     <row r="8" spans="1:15" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>99</v>
+        <v>35</v>
       </c>
       <c r="B8" s="3">
         <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>100</v>
+        <v>29</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="3" t="s">
-        <v>101</v>
+        <v>30</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="3" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>103</v>
+        <v>37</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="8" t="s">
-        <v>104</v>
+      <c r="L8" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
@@ -1561,25 +1147,25 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>105</v>
+        <v>39</v>
       </c>
       <c r="B9" s="3">
         <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>106</v>
+        <v>29</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="3" t="s">
-        <v>107</v>
+        <v>30</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="3" t="s">
-        <v>108</v>
+        <v>40</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>109</v>
+        <v>32</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -1590,25 +1176,25 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>110</v>
+        <v>41</v>
       </c>
       <c r="B10" s="3">
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>111</v>
+        <v>29</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="3" t="s">
-        <v>112</v>
+        <v>30</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="3" t="s">
-        <v>113</v>
+        <v>42</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>114</v>
+        <v>43</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="2"/>
@@ -1619,18 +1205,18 @@
     </row>
     <row r="11" spans="1:15" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>115</v>
+        <v>44</v>
       </c>
       <c r="B11" s="3">
         <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>116</v>
+        <v>29</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="3" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -1644,33 +1230,35 @@
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="B12" s="3">
         <v>8</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>119</v>
+        <v>29</v>
       </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="8" t="s">
-        <v>120</v>
+      <c r="E12" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="G12" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="H12" s="3" t="s">
-        <v>122</v>
+        <v>31</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>123</v>
+        <v>32</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>124</v>
+        <v>48</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>125</v>
+        <v>49</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
@@ -1679,27 +1267,27 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>126</v>
+        <v>50</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>127</v>
+        <v>51</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="3" t="s">
-        <v>129</v>
+        <v>52</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="3" t="s">
-        <v>130</v>
+        <v>53</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>131</v>
+        <v>43</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -1710,32 +1298,32 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>132</v>
+        <v>54</v>
       </c>
       <c r="B14" s="3">
         <v>2</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>133</v>
+        <v>51</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>134</v>
+        <v>55</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="3" t="s">
-        <v>135</v>
+        <v>56</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="3" t="s">
-        <v>136</v>
+        <v>57</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>137</v>
+        <v>32</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
-      <c r="L14" s="8" t="s">
-        <v>138</v>
+      <c r="L14" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
@@ -1743,24 +1331,28 @@
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>152</v>
+        <v>59</v>
       </c>
       <c r="B15" s="3">
         <v>2</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>155</v>
+        <v>51</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>156</v>
+        <v>55</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="3" t="s">
-        <v>157</v>
+        <v>56</v>
       </c>
       <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="H15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
@@ -1770,27 +1362,27 @@
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>158</v>
+        <v>61</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>159</v>
+        <v>51</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>160</v>
+        <v>62</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="3" t="s">
-        <v>161</v>
+        <v>62</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="3" t="s">
-        <v>162</v>
+        <v>63</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>163</v>
+        <v>43</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
@@ -1801,27 +1393,27 @@
     </row>
     <row r="17" spans="1:15" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>164</v>
+        <v>64</v>
       </c>
       <c r="B17" s="3">
         <v>3</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>165</v>
+        <v>51</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>166</v>
+        <v>65</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="3" t="s">
-        <v>167</v>
+        <v>66</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="3" t="s">
-        <v>168</v>
+        <v>67</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>169</v>
+        <v>32</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -1832,69 +1424,73 @@
     </row>
     <row r="18" spans="1:15" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>170</v>
+        <v>68</v>
       </c>
       <c r="B18" s="3">
         <v>3</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>171</v>
+        <v>51</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>173</v>
+        <v>65</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="G18" s="4"/>
+        <v>66</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="H18" s="3" t="s">
-        <v>175</v>
+        <v>70</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>176</v>
+        <v>43</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>177</v>
+        <v>71</v>
       </c>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
-      <c r="M18" s="8" t="s">
-        <v>178</v>
+      <c r="M18" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
     </row>
     <row r="19" spans="1:15" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>179</v>
+        <v>73</v>
       </c>
       <c r="B19" s="3">
         <v>1</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>182</v>
+        <v>51</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="G19" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="H19" s="1" t="s">
-        <v>191</v>
+        <v>76</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="J19" s="12" t="s">
-        <v>193</v>
+        <v>43</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
@@ -1904,27 +1500,27 @@
     </row>
     <row r="20" spans="1:15" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>194</v>
+        <v>78</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>195</v>
+        <v>51</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>196</v>
+        <v>79</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="3" t="s">
-        <v>197</v>
+        <v>79</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="3" t="s">
-        <v>198</v>
+        <v>80</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>199</v>
+        <v>32</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -1935,27 +1531,27 @@
     </row>
     <row r="21" spans="1:15" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>200</v>
+        <v>81</v>
       </c>
       <c r="B21" s="3">
         <v>1</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>201</v>
+        <v>51</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>202</v>
+        <v>79</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="3" t="s">
-        <v>203</v>
+        <v>79</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="3" t="s">
-        <v>204</v>
+        <v>80</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>205</v>
+        <v>32</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -1966,27 +1562,27 @@
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>206</v>
+        <v>82</v>
       </c>
       <c r="B22" s="3">
         <v>1</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>207</v>
+        <v>51</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>208</v>
+        <v>79</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="3" t="s">
-        <v>209</v>
+        <v>79</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="3" t="s">
-        <v>210</v>
+        <v>80</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>211</v>
+        <v>43</v>
       </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -1997,35 +1593,37 @@
     </row>
     <row r="23" spans="1:15" ht="15.75" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>212</v>
+        <v>83</v>
       </c>
       <c r="B23" s="3">
         <v>1</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>213</v>
+        <v>51</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>215</v>
+        <v>84</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="G23" s="4"/>
+        <v>84</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="H23" s="3" t="s">
-        <v>217</v>
+        <v>86</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>218</v>
+        <v>87</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>219</v>
+        <v>88</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>220</v>
+        <v>89</v>
       </c>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
@@ -2034,108 +1632,106 @@
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>221</v>
+        <v>90</v>
       </c>
       <c r="B24" s="3">
         <v>4</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>222</v>
+        <v>51</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>215</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="E24" s="4"/>
       <c r="F24" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>273</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="G24" s="4"/>
       <c r="H24" s="3" t="s">
-        <v>225</v>
+        <v>31</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>226</v>
+        <v>32</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="L24" s="13" t="s">
-        <v>228</v>
+        <v>93</v>
+      </c>
+      <c r="K24" s="4"/>
+      <c r="L24" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="M24" s="15" t="s">
-        <v>274</v>
-      </c>
-      <c r="N24" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="O24" s="14" t="s">
-        <v>272</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>229</v>
+        <v>95</v>
       </c>
       <c r="B25" s="3">
         <v>4</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>230</v>
+        <v>51</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>231</v>
+        <v>91</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="3" t="s">
-        <v>232</v>
+        <v>92</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="3" t="s">
-        <v>233</v>
+        <v>96</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>234</v>
+        <v>43</v>
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
+      <c r="L25" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="M25" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>235</v>
+        <v>99</v>
       </c>
       <c r="B26" s="3">
         <v>4</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>236</v>
+        <v>51</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>237</v>
+        <v>91</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="3" t="s">
-        <v>238</v>
+        <v>92</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="3" t="s">
-        <v>239</v>
+        <v>100</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
@@ -2143,27 +1739,27 @@
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>241</v>
+        <v>103</v>
       </c>
       <c r="B27" s="3">
         <v>4</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>242</v>
+        <v>51</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>243</v>
+        <v>91</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3" t="s">
-        <v>244</v>
+        <v>92</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="3" t="s">
-        <v>245</v>
+        <v>104</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>246</v>
+        <v>43</v>
       </c>
       <c r="J27" s="4"/>
       <c r="K27" s="2"/>
@@ -2174,58 +1770,60 @@
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>247</v>
+        <v>105</v>
       </c>
       <c r="B28" s="3">
         <v>4</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>248</v>
+        <v>51</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>249</v>
+        <v>91</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="3" t="s">
-        <v>250</v>
+        <v>92</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="3" t="s">
-        <v>251</v>
+        <v>31</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>252</v>
+        <v>37</v>
       </c>
       <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
+      <c r="K28" s="3"/>
       <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
+      <c r="M28" s="10" t="s">
+        <v>106</v>
+      </c>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
     </row>
     <row r="29" spans="1:15" ht="15.75" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>253</v>
+        <v>107</v>
       </c>
       <c r="B29" s="3">
         <v>4</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>254</v>
+        <v>51</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>255</v>
+        <v>91</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="3" t="s">
-        <v>256</v>
+        <v>92</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="3" t="s">
-        <v>257</v>
+        <v>104</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>258</v>
+        <v>43</v>
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
@@ -2236,30 +1834,30 @@
     </row>
     <row r="30" spans="1:15" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>259</v>
+        <v>108</v>
       </c>
       <c r="B30" s="3">
         <v>5</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>260</v>
+        <v>51</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>261</v>
+        <v>109</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="3" t="s">
-        <v>262</v>
+        <v>110</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="3" t="s">
-        <v>263</v>
+        <v>111</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>264</v>
+        <v>43</v>
       </c>
       <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
+      <c r="K30" s="3"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
@@ -2267,30 +1865,32 @@
     </row>
     <row r="31" spans="1:15" ht="15.75" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>265</v>
+        <v>112</v>
       </c>
       <c r="B31" s="3">
         <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>266</v>
+        <v>51</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>267</v>
+        <v>113</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="3" t="s">
-        <v>268</v>
+        <v>113</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="3" t="s">
-        <v>269</v>
+        <v>114</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>270</v>
+        <v>37</v>
       </c>
       <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
+      <c r="K31" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
@@ -2307,7 +1907,7 @@
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
+      <c r="K32" s="3"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
@@ -2341,7 +1941,7 @@
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
+      <c r="K34" s="3"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
@@ -2902,11 +2502,12 @@
     <hyperlink ref="E19" r:id="rId7"/>
     <hyperlink ref="E23" r:id="rId8"/>
     <hyperlink ref="L24" r:id="rId9"/>
-    <hyperlink ref="M24" r:id="rId10" display="http://www.TannerLong.com//"/>
-    <hyperlink ref="E24" r:id="rId11"/>
+    <hyperlink ref="M24" r:id="rId10"/>
+    <hyperlink ref="L25" r:id="rId11"/>
+    <hyperlink ref="M25" r:id="rId12"/>
+    <hyperlink ref="M28" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2932,84 +2533,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>46</v>
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="7">
+      <c r="A2" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="13">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>66</v>
+      <c r="C2" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A3" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="7">
+      <c r="A3" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="13">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>79</v>
+      <c r="C3" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1"/>
@@ -3051,50 +2652,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>61</v>
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1"/>
@@ -3138,50 +2739,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A1" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>83</v>
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1"/>
@@ -3225,50 +2826,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A1" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>154</v>
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1"/>
@@ -3312,36 +2913,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A1" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>184</v>
+      <c r="A1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A2" s="6" t="s">
-        <v>185</v>
+      <c r="A2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A3" s="6" t="s">
-        <v>186</v>
+      <c r="A3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A4" s="6" t="s">
-        <v>187</v>
+      <c r="A4" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A5" s="6" t="s">
-        <v>188</v>
+      <c r="A5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A6" s="6" t="s">
-        <v>189</v>
+      <c r="A6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1"/>

</xml_diff>